<commit_message>
commit and pushed by krishna on 7/4/23
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\Vtiger.WCSM23.AutomationFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D33AF382-5383-42E0-83F6-920CC7AEB521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A09D9E4-DFAA-4CB7-8B89-817E945B7989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
     <sheet name="Contacts" sheetId="2" r:id="rId3"/>
     <sheet name="MultipleData" sheetId="3" r:id="rId4"/>
+    <sheet name="CustomerDetails" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="50">
   <si>
     <t>TC_ID</t>
   </si>
@@ -154,6 +155,30 @@
   </si>
   <si>
     <t>Healthcare</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>CustomerDescription</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Test Lead</t>
+  </si>
+  <si>
+    <t>Vamsi</t>
+  </si>
+  <si>
+    <t>Devloer</t>
+  </si>
+  <si>
+    <t>Shyam</t>
+  </si>
+  <si>
+    <t>ManualTester</t>
   </si>
 </sst>
 </file>
@@ -749,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F6C2C5-1C00-4260-A589-B6320297F9C9}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -810,4 +835,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63619EBE-9D77-4119-BE54-8574B32EBA23}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>